<commit_message>
Added more methods to help with main
</commit_message>
<xml_diff>
--- a/ExcelFiles/WGUPS Package File.xlsx
+++ b/ExcelFiles/WGUPS Package File.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/specter/PycharmProjects/C950/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/specter/C950/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74BE71D-DEAE-EA45-B48B-3E5146D92AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13676F58-A57E-2348-A39D-60CBD745E7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="500" windowWidth="24680" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="24640" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,30 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="50">
   <si>
     <t>WGUPS Package File</t>
   </si>
@@ -212,90 +189,6 @@
   </si>
   <si>
     <t>'4001 S700 E', '3595 Main St', '3365 S 900 W', '1488 4800 S', '2010 W 500 S', '233 Canyon Rd', '300 State St', '195 W Oakland Ave', '177 W Price Ave', '380 W 2880 S', '1330 2100 S', '4300 S 1300 E', '4580 S 2300 E', '4001 S700 E']</t>
-  </si>
-  <si>
-    <t>4001 S700 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3595 Main St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3365 S 900 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1488 4800 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2010 W 500 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 233 Canyon Rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 300 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 195 W Oakland Ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 177 W Price Ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 380 W 2880 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1330 2100 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4300 S 1300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4580 S 2300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4001 S700 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2530 S 500 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2835 Main St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6351 S900 East</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5383 S900 E#104</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3148 S 1100 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3060 Lester St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1060 Dalton Ave S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 410 S State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5025 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2600 Taylorsville Blvd</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5100 S2700 West</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 600 E 900 South</t>
-  </si>
-  <si>
-    <t>Deadline</t>
   </si>
 </sst>
 </file>
@@ -378,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -419,7 +312,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -1869,509 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFD2EE6-FBAD-0C4D-A861-F537FDB5344C}">
-  <dimension ref="A1:P50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3:A16">TRANSPOSE(TRIM(A1:N1))</f>
-        <v>4001 S700 E</v>
-      </c>
-      <c r="B3" t="e">
-        <f>_xlfn.XLOOKUP(A3,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <v>3595 Main St</v>
-      </c>
-      <c r="B4">
-        <f>_xlfn.XLOOKUP(A4,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <v>3365 S 900 W</v>
-      </c>
-      <c r="B5">
-        <f>_xlfn.XLOOKUP(A5,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
-        <v>1488 4800 S</v>
-      </c>
-      <c r="B6" t="str">
-        <f>_xlfn.XLOOKUP(A6,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
-        <v>2010 W 500 S</v>
-      </c>
-      <c r="B7">
-        <f>_xlfn.XLOOKUP(A7,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
-        <v>233 Canyon Rd</v>
-      </c>
-      <c r="B8" t="str">
-        <f>_xlfn.XLOOKUP(A8,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" t="str">
-        <v>300 State St</v>
-      </c>
-      <c r="B9" t="str">
-        <f>_xlfn.XLOOKUP(A9,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
-        <v>195 W Oakland Ave</v>
-      </c>
-      <c r="B10">
-        <f>_xlfn.XLOOKUP(A10,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="str">
-        <v>177 W Price Ave</v>
-      </c>
-      <c r="B11" t="str">
-        <f>_xlfn.XLOOKUP(A11,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
-        <v>380 W 2880 S</v>
-      </c>
-      <c r="B12" t="str">
-        <f>_xlfn.XLOOKUP(A12,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
-        <v>1330 2100 S</v>
-      </c>
-      <c r="B13" t="str">
-        <f>_xlfn.XLOOKUP(A13,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
-        <v>4300 S 1300 E</v>
-      </c>
-      <c r="B14">
-        <f>_xlfn.XLOOKUP(A14,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
-        <v>4580 S 2300 E</v>
-      </c>
-      <c r="B15">
-        <f>_xlfn.XLOOKUP(A15,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="str">
-        <v>4001 S700 E</v>
-      </c>
-      <c r="B16" t="e">
-        <f>_xlfn.XLOOKUP(A16,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" t="s">
-        <v>70</v>
-      </c>
-      <c r="K21" t="s">
-        <v>54</v>
-      </c>
-      <c r="L21" t="s">
-        <v>56</v>
-      </c>
-      <c r="M21" t="s">
-        <v>71</v>
-      </c>
-      <c r="N21" t="s">
-        <v>59</v>
-      </c>
-      <c r="O21" t="s">
-        <v>51</v>
-      </c>
-      <c r="P21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" t="str" cm="1">
-        <f t="array" ref="A23:A38">TRANSPOSE(TRIM(A21:P21))</f>
-        <v>4001 S700 E</v>
-      </c>
-      <c r="B23" t="e">
-        <f>_xlfn.XLOOKUP(A23,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <v>1330 2100 S</v>
-      </c>
-      <c r="B24" t="str">
-        <f>_xlfn.XLOOKUP(A24,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
-        <v>2530 S 500 E</v>
-      </c>
-      <c r="B25" t="str">
-        <f>_xlfn.XLOOKUP(A25,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
-        <v>2835 Main St</v>
-      </c>
-      <c r="B26" t="str">
-        <f>_xlfn.XLOOKUP(A26,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
-        <v>6351 S900 East</v>
-      </c>
-      <c r="B27" t="e">
-        <f>_xlfn.XLOOKUP(A27,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
-        <v>5383 S900 E#104</v>
-      </c>
-      <c r="B28" t="e">
-        <f>_xlfn.XLOOKUP(A28,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" t="str">
-        <v>3365 S 900 W</v>
-      </c>
-      <c r="B29">
-        <f>_xlfn.XLOOKUP(A29,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" t="str">
-        <v>3148 S 1100 W</v>
-      </c>
-      <c r="B30" t="str">
-        <f>_xlfn.XLOOKUP(A30,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" t="str">
-        <v>3060 Lester St</v>
-      </c>
-      <c r="B31">
-        <f>_xlfn.XLOOKUP(A31,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
-        <v>1060 Dalton Ave S</v>
-      </c>
-      <c r="B32" t="str">
-        <f>_xlfn.XLOOKUP(A32,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
-        <v>2010 W 500 S</v>
-      </c>
-      <c r="B33">
-        <f>_xlfn.XLOOKUP(A33,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <v>300 State St</v>
-      </c>
-      <c r="B34" t="str">
-        <f>_xlfn.XLOOKUP(A34,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
-        <v>410 S State St</v>
-      </c>
-      <c r="B35" t="str">
-        <f>_xlfn.XLOOKUP(A35,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <v>380 W 2880 S</v>
-      </c>
-      <c r="B36" t="str">
-        <f>_xlfn.XLOOKUP(A36,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>EOD</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="str">
-        <v>3595 Main St</v>
-      </c>
-      <c r="B37">
-        <f>_xlfn.XLOOKUP(A37,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="str">
-        <v>4001 S700 E</v>
-      </c>
-      <c r="B38" t="e">
-        <f>_xlfn.XLOOKUP(A38,Sheet1!$B$9:$B$48,Sheet1!$F$9:$F$48)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" t="s">
-        <v>56</v>
-      </c>
-      <c r="G41" t="s">
-        <v>76</v>
-      </c>
-      <c r="H41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" t="str" cm="1">
-        <f t="array" ref="A43:A50">TRANSPOSE(TRIM(A41:H41))</f>
-        <v>4001 S700 E</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="str">
-        <v>5025 State St</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="str">
-        <v>2600 Taylorsville Blvd</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" t="str">
-        <v>5100 S2700 West</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" t="str">
-        <v>3575 W Valley Central Station bus Loop</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
-        <v>300 State St</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <v>600 E 900 South</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <v>4001 S700 E</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>Objective</Value>
-    </Assessment_x0020_Type>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67abd11da167d8eab610c259a823e4c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d3ab84303ed41503c975572ff37e680" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2809,33 +2199,53 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>Objective</Value>
+    </Assessment_x0020_Type>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A0206-F67A-481E-AE05-AF5EAD7E6628}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2853,4 +2263,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>